<commit_message>
search box resizing implemented
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/testing.xlsx
+++ b/Content Engineer Studio/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03CC31E-684D-41B6-AD5E-7963849D6465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17413425-A6AD-4A8B-B70E-E91D73F4ECB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27432" yWindow="3000" windowWidth="22344" windowHeight="12660" xr2:uid="{F7E6B734-54B9-435D-8347-4E48591D8B7F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Korrekter Flow/FAQ</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>asfd</t>
-  </si>
-  <si>
-    <t>afer</t>
   </si>
 </sst>
 </file>
@@ -444,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31EDC131-CAFD-4FC1-A565-3F5D4E455030}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,7 +459,7 @@
     <col min="9" max="9" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -485,7 +482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -507,26 +504,23 @@
       <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
tab switching and exporting implemented.
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/testing.xlsx
+++ b/Content Engineer Studio/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17413425-A6AD-4A8B-B70E-E91D73F4ECB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E003C2-7891-4B77-A0AA-5CC952B1671F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27432" yWindow="3000" windowWidth="22344" windowHeight="12660" xr2:uid="{F7E6B734-54B9-435D-8347-4E48591D8B7F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="8">
   <si>
     <t>Korrekter Flow/FAQ</t>
   </si>
@@ -55,25 +55,7 @@
     <t>Visum und Details</t>
   </si>
   <si>
-    <t>geht so</t>
-  </si>
-  <si>
     <t>111111111111111d54</t>
-  </si>
-  <si>
-    <t>xxxxxxxxx</t>
-  </si>
-  <si>
-    <t>aaaaaa</t>
-  </si>
-  <si>
-    <t>fdsfsdf</t>
-  </si>
-  <si>
-    <t>gawrefasdf</t>
-  </si>
-  <si>
-    <t>asfd</t>
   </si>
 </sst>
 </file>
@@ -441,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31EDC131-CAFD-4FC1-A565-3F5D4E455030}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,45 +466,167 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
btn_right_2 working correctly again.
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/testing.xlsx
+++ b/Content Engineer Studio/testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E976E8-1B95-4FF6-A168-51D97292E037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48F0EF6-14C6-4CFD-AD38-4A07A9C64850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="348" yWindow="744" windowWidth="22104" windowHeight="12660" xr2:uid="{F7E6B734-54B9-435D-8347-4E48591D8B7F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="19">
   <si>
     <t>Korrekter Flow/FAQ</t>
   </si>
@@ -61,7 +61,34 @@
     <t>test</t>
   </si>
   <si>
-    <t>naja</t>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>hmm</t>
+  </si>
+  <si>
+    <t>bissifiel</t>
+  </si>
+  <si>
+    <t>aufirohrum</t>
+  </si>
+  <si>
+    <t>adfg</t>
+  </si>
+  <si>
+    <t>arhf</t>
+  </si>
+  <si>
+    <t>haerfg</t>
+  </si>
+  <si>
+    <t>ashfrfdg</t>
+  </si>
+  <si>
+    <t>asdfhpoh</t>
+  </si>
+  <si>
+    <t>apfsogh</t>
   </si>
 </sst>
 </file>
@@ -431,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31EDC131-CAFD-4FC1-A565-3F5D4E455030}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,25 +507,52 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
colorize and open_links implemented
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/testing.xlsx
+++ b/Content Engineer Studio/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48F0EF6-14C6-4CFD-AD38-4A07A9C64850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254960FC-CEE2-4D8C-91E5-C918AE25F46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="744" windowWidth="22104" windowHeight="12660" xr2:uid="{F7E6B734-54B9-435D-8347-4E48591D8B7F}"/>
+    <workbookView xWindow="-29544" yWindow="1440" windowWidth="22104" windowHeight="12660" xr2:uid="{F7E6B734-54B9-435D-8347-4E48591D8B7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="12">
   <si>
     <t>Korrekter Flow/FAQ</t>
   </si>
@@ -58,37 +58,20 @@
     <t>111111111111111d54</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>xxx</t>
-  </si>
-  <si>
-    <t>hmm</t>
-  </si>
-  <si>
-    <t>bissifiel</t>
-  </si>
-  <si>
-    <t>aufirohrum</t>
-  </si>
-  <si>
-    <t>adfg</t>
-  </si>
-  <si>
-    <t>arhf</t>
-  </si>
-  <si>
-    <t>haerfg</t>
-  </si>
-  <si>
-    <t>ashfrfdg</t>
-  </si>
-  <si>
-    <t>asdfhpoh</t>
-  </si>
-  <si>
-    <t>apfsogh</t>
+    <t>Ham &amp; Potato Soup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Bot hat das Anliegen richtig verstanden. Das Anliegen konnte jedoch nicht gelöst werden. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+I am well, thank you.
+I am not sure, but it must be a lot.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+What are you doing¿?
+Interesting. Tell me more about you.</t>
   </si>
 </sst>
 </file>
@@ -130,16 +113,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -458,20 +440,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31EDC131-CAFD-4FC1-A565-3F5D4E455030}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" customWidth="1"/>
-    <col min="2" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" customWidth="1"/>
-    <col min="6" max="6" width="19.21875" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" customWidth="1"/>
-    <col min="8" max="8" width="25.77734375" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" style="2" customWidth="1"/>
+    <col min="2" max="3" width="21" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="25.77734375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -481,10 +464,10 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -497,201 +480,180 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Attempting to implement auto highlighting
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/testing.xlsx
+++ b/Content Engineer Studio/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254960FC-CEE2-4D8C-91E5-C918AE25F46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D1F2F8-3299-43C1-88EB-30EFD8E183EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29544" yWindow="1440" windowWidth="22104" windowHeight="12660" xr2:uid="{F7E6B734-54B9-435D-8347-4E48591D8B7F}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="396" windowWidth="22104" windowHeight="12660" xr2:uid="{F7E6B734-54B9-435D-8347-4E48591D8B7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
   <si>
     <t>Korrekter Flow/FAQ</t>
   </si>
@@ -58,10 +58,7 @@
     <t>111111111111111d54</t>
   </si>
   <si>
-    <t>Ham &amp; Potato Soup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Der Bot hat das Anliegen richtig verstanden. Das Anliegen konnte jedoch nicht gelöst werden. </t>
+    <t>Mediterranean Tuna Steaks</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -70,8 +67,15 @@
   </si>
   <si>
     <t xml:space="preserve">
-What are you doing¿?
-Interesting. Tell me more about you.</t>
+What about the ups?
+That's good.
+Haha, well, let's just say you don't want to be involved with i</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Es hat nicht gut geklappt, da der Bot das Anliegen nicht richtig erkannt hat. FAQ xy wäre besser.0420000000</t>
   </si>
 </sst>
 </file>
@@ -87,7 +91,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,6 +101,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -113,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -122,6 +132,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -441,7 +454,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,7 +493,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -488,171 +501,177 @@
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="3">
+        <v>420000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
new dialog multi threading implemented
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/testing.xlsx
+++ b/Content Engineer Studio/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F1BE9D-1B37-42E5-9CD7-75393219A71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD41A84-FEC6-4419-AAF3-C12BE1FF824B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="744" windowWidth="22104" windowHeight="12660" xr2:uid="{F7E6B734-54B9-435D-8347-4E48591D8B7F}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="396" windowWidth="22104" windowHeight="12660" xr2:uid="{F7E6B734-54B9-435D-8347-4E48591D8B7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding FaqAutoSearch to StackedWidget
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/testing.xlsx
+++ b/Content Engineer Studio/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B98966B-EEC6-4D7C-BFFE-455E6E845B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D90581-2454-4E01-8FD4-3FA2DD9CEC0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="396" windowWidth="22104" windowHeight="12660" xr2:uid="{F7E6B734-54B9-435D-8347-4E48591D8B7F}"/>
+    <workbookView xWindow="348" yWindow="744" windowWidth="22104" windowHeight="12660" xr2:uid="{F7E6B734-54B9-435D-8347-4E48591D8B7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
moved chat selection to subclass
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/testing.xlsx
+++ b/Content Engineer Studio/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB449878-AEAF-40C5-897D-E061963A1E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300867CF-15A0-4D08-9B7B-6A4A08EA4FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="300" windowWidth="22104" windowHeight="12660" xr2:uid="{F7E6B734-54B9-435D-8347-4E48591D8B7F}"/>
+    <workbookView xWindow="0" yWindow="396" windowWidth="22104" windowHeight="12660" xr2:uid="{F7E6B734-54B9-435D-8347-4E48591D8B7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="15">
   <si>
     <t>Korrekter Flow/FAQ</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Es hat nicht gut geklappt, da der Bot das Anliegen nicht richtig erkannt hat. FAQ xy wäre besser.0420000000</t>
+  </si>
+  <si>
+    <t>We will we will.</t>
+  </si>
+  <si>
+    <t>Rock you.</t>
   </si>
 </sst>
 </file>
@@ -527,6 +533,12 @@
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">

</xml_diff>

<commit_message>
added refs to class
</commit_message>
<xml_diff>
--- a/Content Engineer Studio/testing.xlsx
+++ b/Content Engineer Studio/testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\Content Engineer Studio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB449878-AEAF-40C5-897D-E061963A1E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9483C6-F4B3-412B-9524-BC853F87BCD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="300" windowWidth="22104" windowHeight="12660" xr2:uid="{F7E6B734-54B9-435D-8347-4E48591D8B7F}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="756" windowWidth="14244" windowHeight="7776" xr2:uid="{F7E6B734-54B9-435D-8347-4E48591D8B7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="8">
   <si>
     <t>Korrekter Flow/FAQ</t>
   </si>
@@ -56,26 +56,6 @@
   </si>
   <si>
     <t>111111111111111d54</t>
-  </si>
-  <si>
-    <t>Mediterranean Tuna Steaks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-I am well, thank you.
-I am not sure, but it must be a lot.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-What about the ups?
-That's good.
-Haha, well, let's just say you don't want to be involved with i</t>
-  </si>
-  <si>
-    <t>Details</t>
-  </si>
-  <si>
-    <t>Es hat nicht gut geklappt, da der Bot das Anliegen nicht richtig erkannt hat. FAQ xy wäre besser.0420000000</t>
   </si>
 </sst>
 </file>
@@ -91,7 +71,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,12 +81,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -123,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -132,9 +106,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -453,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31EDC131-CAFD-4FC1-A565-3F5D4E455030}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,24 +464,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -536,9 +492,6 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="F7" s="3">
-        <v>420000000</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>